<commit_message>
update project stucture plan
</commit_message>
<xml_diff>
--- a/doc/Projektablaufplan.xlsx
+++ b/doc/Projektablaufplan.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5828D5DF-B9E1-4468-AC16-E0679F4A87D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE594A67-4B5D-4159-A297-24A49E7B4F1E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="2124" windowWidth="17280" windowHeight="9060" tabRatio="415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Gantt" sheetId="11" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="102">
   <si>
     <t>Erstellen Sie auf diesem Arbeitsblatt ein Gantt-Diagramm.
 Geben Sie den Titel dieses Projekts in Zelle B1 ein. 
@@ -371,6 +371,9 @@
   </si>
   <si>
     <t>Überarbeitung</t>
+  </si>
+  <si>
+    <t>Seiten erstellen, Design überarbeiten</t>
   </si>
 </sst>
 </file>
@@ -1169,7 +1172,7 @@
       <alignment horizontal="left" wrapText="1" indent="2"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1343,9 +1346,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="9" applyFont="1" applyFill="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3051,16 +3051,16 @@
                 <c:formatCode>[hh]:mm</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.78125000000000022</c:v>
+                  <c:v>0.87847222222222254</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.60416666666666696</c:v>
+                  <c:v>0.6805555555555558</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.86111111111111127</c:v>
+                  <c:v>0.93750000000000022</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.55208333333333348</c:v>
+                  <c:v>0.76736111111111116</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4227,7 +4227,7 @@
   <dimension ref="A1:BO57"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="73" zoomScaleNormal="145" zoomScalePageLayoutView="85" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="5" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
@@ -4290,30 +4290,30 @@
       <c r="A2" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="86"/>
+      <c r="B2" s="85"/>
       <c r="C2" s="18"/>
       <c r="D2" s="18"/>
       <c r="E2" s="18"/>
-      <c r="F2" s="80" t="s">
+      <c r="F2" s="79" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="81"/>
-      <c r="H2" s="83">
+      <c r="G2" s="80"/>
+      <c r="H2" s="82">
         <v>44097</v>
       </c>
-      <c r="I2" s="84"/>
-      <c r="J2" s="85"/>
+      <c r="I2" s="83"/>
+      <c r="J2" s="84"/>
       <c r="K2" s="20"/>
     </row>
     <row r="3" spans="1:67" ht="29.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="86"/>
-      <c r="F3" s="80" t="s">
+      <c r="B3" s="85"/>
+      <c r="F3" s="79" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="81"/>
+      <c r="G3" s="80"/>
       <c r="H3" s="41">
         <v>0</v>
       </c>
@@ -4403,16 +4403,16 @@
       <c r="A4" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="82"/>
-      <c r="C4" s="82"/>
-      <c r="D4" s="82"/>
-      <c r="E4" s="82"/>
-      <c r="F4" s="82"/>
-      <c r="G4" s="82"/>
-      <c r="H4" s="82"/>
-      <c r="I4" s="82"/>
-      <c r="J4" s="82"/>
-      <c r="K4" s="82"/>
+      <c r="B4" s="81"/>
+      <c r="C4" s="81"/>
+      <c r="D4" s="81"/>
+      <c r="E4" s="81"/>
+      <c r="F4" s="81"/>
+      <c r="G4" s="81"/>
+      <c r="H4" s="81"/>
+      <c r="I4" s="81"/>
+      <c r="J4" s="81"/>
+      <c r="K4" s="81"/>
       <c r="L4" s="42">
         <f ca="1">IFERROR(Projekt_Start+Scroll_Schrittweite,TODAY())</f>
         <v>44097</v>
@@ -6706,7 +6706,7 @@
       <c r="B16" s="53" t="s">
         <v>88</v>
       </c>
-      <c r="C16" s="79">
+      <c r="C16" s="78">
         <v>0.41666666666666669</v>
       </c>
       <c r="D16" s="59" t="str">
@@ -6791,7 +6791,7 @@
       <c r="B17" s="53" t="s">
         <v>75</v>
       </c>
-      <c r="C17" s="79">
+      <c r="C17" s="78">
         <v>0.41666666666666669</v>
       </c>
       <c r="D17" s="59" t="str">
@@ -7466,7 +7466,7 @@
         <v>0</v>
       </c>
       <c r="H24" s="29"/>
-      <c r="I24" s="77"/>
+      <c r="I24" s="76"/>
       <c r="J24" s="30">
         <f>IF(Meilensteine[[#This Row],[Kategorie]]="Meilenstein",1,_xlfn.DAYS(Meilensteine[[#This Row],[Ende]],Meilensteine[[#This Row],[Start]]))</f>
         <v>0</v>
@@ -7626,7 +7626,7 @@
       <c r="B26" s="53" t="s">
         <v>77</v>
       </c>
-      <c r="C26" s="79">
+      <c r="C26" s="78">
         <v>0.20833333333333334</v>
       </c>
       <c r="D26" s="59" t="str">
@@ -7711,7 +7711,7 @@
       <c r="B27" s="53" t="s">
         <v>78</v>
       </c>
-      <c r="C27" s="79">
+      <c r="C27" s="78">
         <v>0.33333333333333331</v>
       </c>
       <c r="D27" s="59" t="str">
@@ -7796,7 +7796,7 @@
       <c r="B28" s="53" t="s">
         <v>82</v>
       </c>
-      <c r="C28" s="79">
+      <c r="C28" s="78">
         <v>0.25</v>
       </c>
       <c r="D28" s="59" t="str">
@@ -7881,7 +7881,7 @@
       <c r="B29" s="53" t="s">
         <v>79</v>
       </c>
-      <c r="C29" s="79">
+      <c r="C29" s="78">
         <v>0.41666666666666669</v>
       </c>
       <c r="D29" s="59" t="str">
@@ -7963,10 +7963,10 @@
     </row>
     <row r="30" spans="1:67" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A30" s="14"/>
-      <c r="B30" s="78" t="s">
+      <c r="B30" s="77" t="s">
         <v>53</v>
       </c>
-      <c r="C30" s="79"/>
+      <c r="C30" s="78"/>
       <c r="D30" s="59"/>
       <c r="E30" s="31"/>
       <c r="F30" s="31"/>
@@ -8037,7 +8037,7 @@
       <c r="B31" s="53" t="s">
         <v>99</v>
       </c>
-      <c r="C31" s="79"/>
+      <c r="C31" s="78"/>
       <c r="D31" s="59">
         <f>IF(VLOOKUP(Meilensteine[[#This Row],[Arbeitspaket]],Übersicht!B:G,6,FALSE)=0,"",VLOOKUP(Meilensteine[[#This Row],[Arbeitspaket]],Übersicht!B:G,6,FALSE))</f>
         <v>0.14930555555555555</v>
@@ -8114,9 +8114,9 @@
       <c r="C32" s="68">
         <v>0.41666666666666669</v>
       </c>
-      <c r="D32" s="59" t="str">
+      <c r="D32" s="59">
         <f>IF(VLOOKUP(Meilensteine[[#This Row],[Arbeitspaket]],Übersicht!B:G,6,FALSE)=0,"",VLOOKUP(Meilensteine[[#This Row],[Arbeitspaket]],Übersicht!B:G,6,FALSE))</f>
-        <v/>
+        <v>0.1388888888888889</v>
       </c>
       <c r="E32" s="31" t="s">
         <v>11</v>
@@ -8127,7 +8127,7 @@
       <c r="G32" s="28">
         <v>0</v>
       </c>
-      <c r="H32" s="77"/>
+      <c r="H32" s="76"/>
       <c r="I32" s="29"/>
       <c r="J32" s="30">
         <f>IF(Meilensteine[[#This Row],[Kategorie]]="Meilenstein",1,_xlfn.DAYS(Meilensteine[[#This Row],[Ende]],Meilensteine[[#This Row],[Start]]))</f>
@@ -8211,7 +8211,7 @@
       <c r="B33" s="53" t="s">
         <v>89</v>
       </c>
-      <c r="C33" s="79">
+      <c r="C33" s="78">
         <v>0.16666666666666666</v>
       </c>
       <c r="D33" s="59" t="str">
@@ -8227,7 +8227,7 @@
       <c r="G33" s="28">
         <v>0</v>
       </c>
-      <c r="H33" s="77"/>
+      <c r="H33" s="76"/>
       <c r="I33" s="29"/>
       <c r="J33" s="30">
         <f>IF(Meilensteine[[#This Row],[Kategorie]]="Meilenstein",1,_xlfn.DAYS(Meilensteine[[#This Row],[Ende]],Meilensteine[[#This Row],[Start]]))</f>
@@ -8296,7 +8296,7 @@
       <c r="B34" s="53" t="s">
         <v>83</v>
       </c>
-      <c r="C34" s="79">
+      <c r="C34" s="78">
         <v>0.29166666666666669</v>
       </c>
       <c r="D34" s="59" t="str">
@@ -8312,7 +8312,7 @@
       <c r="G34" s="28">
         <v>0</v>
       </c>
-      <c r="H34" s="77"/>
+      <c r="H34" s="76"/>
       <c r="I34" s="29"/>
       <c r="J34" s="30">
         <f>IF(Meilensteine[[#This Row],[Kategorie]]="Meilenstein",1,_xlfn.DAYS(Meilensteine[[#This Row],[Ende]],Meilensteine[[#This Row],[Start]]))</f>
@@ -8381,7 +8381,7 @@
       <c r="B35" s="53" t="s">
         <v>84</v>
       </c>
-      <c r="C35" s="79">
+      <c r="C35" s="78">
         <v>0.125</v>
       </c>
       <c r="D35" s="59" t="str">
@@ -8397,7 +8397,7 @@
       <c r="G35" s="28">
         <v>0</v>
       </c>
-      <c r="H35" s="77"/>
+      <c r="H35" s="76"/>
       <c r="I35" s="29"/>
       <c r="J35" s="30">
         <f>IF(Meilensteine[[#This Row],[Kategorie]]="Meilenstein",1,_xlfn.DAYS(Meilensteine[[#This Row],[Ende]],Meilensteine[[#This Row],[Start]]))</f>
@@ -8466,7 +8466,7 @@
       <c r="B36" s="53" t="s">
         <v>85</v>
       </c>
-      <c r="C36" s="79">
+      <c r="C36" s="78">
         <v>0.33333333333333331</v>
       </c>
       <c r="D36" s="59" t="str">
@@ -8482,7 +8482,7 @@
       <c r="G36" s="28">
         <v>0</v>
       </c>
-      <c r="H36" s="77"/>
+      <c r="H36" s="76"/>
       <c r="I36" s="29"/>
       <c r="J36" s="30">
         <f>IF(Meilensteine[[#This Row],[Kategorie]]="Meilenstein",1,_xlfn.DAYS(Meilensteine[[#This Row],[Ende]],Meilensteine[[#This Row],[Start]]))</f>
@@ -8551,7 +8551,7 @@
       <c r="B37" s="53" t="s">
         <v>86</v>
       </c>
-      <c r="C37" s="79">
+      <c r="C37" s="78">
         <v>0.16666666666666666</v>
       </c>
       <c r="D37" s="59" t="str">
@@ -8567,7 +8567,7 @@
       <c r="G37" s="28">
         <v>0</v>
       </c>
-      <c r="H37" s="77"/>
+      <c r="H37" s="76"/>
       <c r="I37" s="29"/>
       <c r="J37" s="30">
         <f>IF(Meilensteine[[#This Row],[Kategorie]]="Meilenstein",1,_xlfn.DAYS(Meilensteine[[#This Row],[Ende]],Meilensteine[[#This Row],[Start]]))</f>
@@ -8636,7 +8636,7 @@
       <c r="B38" s="53" t="s">
         <v>87</v>
       </c>
-      <c r="C38" s="79">
+      <c r="C38" s="78">
         <v>0.16666666666666666</v>
       </c>
       <c r="D38" s="59" t="str">
@@ -8652,7 +8652,7 @@
       <c r="G38" s="28">
         <v>0</v>
       </c>
-      <c r="H38" s="77"/>
+      <c r="H38" s="76"/>
       <c r="I38" s="29"/>
       <c r="J38" s="30">
         <f>IF(Meilensteine[[#This Row],[Kategorie]]="Meilenstein",1,_xlfn.DAYS(Meilensteine[[#This Row],[Ende]],Meilensteine[[#This Row],[Start]]))</f>
@@ -9600,7 +9600,7 @@
       </c>
       <c r="D45" s="59">
         <f>IF(VLOOKUP(Meilensteine[[#This Row],[Arbeitspaket]],Übersicht!B:G,6,FALSE)=0,"",VLOOKUP(Meilensteine[[#This Row],[Arbeitspaket]],Übersicht!B:G,6,FALSE))</f>
-        <v>0.10416666666666666</v>
+        <v>0.12499999999999999</v>
       </c>
       <c r="E45" s="31" t="s">
         <v>11</v>
@@ -9773,7 +9773,7 @@
       </c>
       <c r="D47" s="59">
         <f>IF(VLOOKUP(Meilensteine[[#This Row],[Arbeitspaket]],Übersicht!B:G,6,FALSE)=0,"",VLOOKUP(Meilensteine[[#This Row],[Arbeitspaket]],Übersicht!B:G,6,FALSE))</f>
-        <v>0.75000000000000044</v>
+        <v>0.91666666666666696</v>
       </c>
       <c r="E47" s="31" t="s">
         <v>11</v>
@@ -9858,7 +9858,7 @@
       </c>
       <c r="D48" s="59">
         <f>IF(VLOOKUP(Meilensteine[[#This Row],[Arbeitspaket]],Übersicht!B:G,6,FALSE)=0,"",VLOOKUP(Meilensteine[[#This Row],[Arbeitspaket]],Übersicht!B:G,6,FALSE))</f>
-        <v>1.2777777777777781</v>
+        <v>1.4166666666666672</v>
       </c>
       <c r="E48" s="31" t="s">
         <v>11</v>
@@ -9938,7 +9938,7 @@
       <c r="B49" s="53" t="s">
         <v>62</v>
       </c>
-      <c r="C49" s="79">
+      <c r="C49" s="78">
         <v>0.41666666666666669</v>
       </c>
       <c r="D49" s="59" t="str">
@@ -10014,7 +10014,7 @@
       <c r="B50" s="53" t="s">
         <v>95</v>
       </c>
-      <c r="C50" s="79"/>
+      <c r="C50" s="78"/>
       <c r="D50" s="59">
         <f>IF(VLOOKUP(Meilensteine[[#This Row],[Arbeitspaket]],Übersicht!B:G,6,FALSE)=0,"",VLOOKUP(Meilensteine[[#This Row],[Arbeitspaket]],Übersicht!B:G,6,FALSE))</f>
         <v>0.18055555555555558</v>
@@ -10680,7 +10680,7 @@
       </c>
       <c r="D54" s="68">
         <f>SUM(D8:D53)</f>
-        <v>2.7986111111111116</v>
+        <v>3.2638888888888893</v>
       </c>
       <c r="E54" s="69" t="s">
         <v>37</v>
@@ -10691,7 +10691,7 @@
       </c>
       <c r="G54" s="28">
         <f>(Meilensteine[[#This Row],[tatsächlicher Aufwand'[h']]]/Meilensteine[[#This Row],[Aufwandsschätzung'[h']]])</f>
-        <v>0.19412331406551067</v>
+        <v>0.2263969171483623</v>
       </c>
       <c r="H54" s="29"/>
       <c r="I54" s="29"/>
@@ -11171,6 +11171,21 @@
           <xm:sqref>G6:G49 G51:G54</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{BCDF6180-781D-41D4-9F20-293570D1F4B2}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>G50</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="iconSet" priority="73" id="{628A03C6-EE71-4B44-A6BA-69DC45906EA6}">
             <x14:iconSet iconSet="3Stars" showValue="0" custom="1">
               <x14:cfvo type="percent">
@@ -11208,21 +11223,6 @@
           </x14:cfRule>
           <xm:sqref>L7:BO55</xm:sqref>
         </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{BCDF6180-781D-41D4-9F20-293570D1F4B2}">
-            <x14:dataBar minLength="0" maxLength="100" gradient="0">
-              <x14:cfvo type="num">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>G50</xm:sqref>
-        </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
   </extLst>
@@ -11764,11 +11764,11 @@
       </c>
       <c r="F23" s="67">
         <f>SUMIF(Sabrina!B:B,Übersicht!B23,Sabrina!F:F)</f>
-        <v>0</v>
+        <v>0.1388888888888889</v>
       </c>
       <c r="G23" s="67">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.1388888888888889</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.3">
@@ -12052,7 +12052,7 @@
       </c>
       <c r="C35" s="55">
         <f>SUMIF(Jacob!B:B,Übersicht!B35,Jacob!F:F)</f>
-        <v>0.10416666666666666</v>
+        <v>0.12499999999999999</v>
       </c>
       <c r="D35" s="67">
         <f>SUMIF(Roman!B:B,Übersicht!B35,Roman!F:F)</f>
@@ -12068,7 +12068,7 @@
       </c>
       <c r="G35" s="67">
         <f t="shared" si="0"/>
-        <v>0.10416666666666666</v>
+        <v>0.12499999999999999</v>
       </c>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.3">
@@ -12102,23 +12102,23 @@
       </c>
       <c r="C37" s="55">
         <f>SUMIF(Jacob!B:B,Übersicht!B37,Jacob!F:F)</f>
-        <v>0.20833333333333348</v>
+        <v>0.25000000000000011</v>
       </c>
       <c r="D37" s="67">
         <f>SUMIF(Roman!B:B,Übersicht!B37,Roman!F:F)</f>
-        <v>0.20833333333333348</v>
+        <v>0.25000000000000011</v>
       </c>
       <c r="E37" s="67">
         <f>SUMIF(Michi!B:B,Übersicht!B37,Michi!F:F)</f>
-        <v>0.20833333333333348</v>
+        <v>0.25000000000000011</v>
       </c>
       <c r="F37" s="67">
         <f>SUMIF(Sabrina!B:B,Übersicht!B37,Sabrina!F:F)</f>
-        <v>0.12500000000000006</v>
+        <v>0.16666666666666669</v>
       </c>
       <c r="G37" s="67">
         <f t="shared" si="0"/>
-        <v>0.75000000000000044</v>
+        <v>0.91666666666666696</v>
       </c>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.3">
@@ -12127,23 +12127,23 @@
       </c>
       <c r="C38" s="55">
         <f>SUMIF(Jacob!B:B,Übersicht!B38,Jacob!F:F)</f>
-        <v>0.31944444444444453</v>
+        <v>0.3541666666666668</v>
       </c>
       <c r="D38" s="67">
         <f>SUMIF(Roman!B:B,Übersicht!B38,Roman!F:F)</f>
-        <v>0.31944444444444453</v>
+        <v>0.3541666666666668</v>
       </c>
       <c r="E38" s="67">
         <f>SUMIF(Michi!B:B,Übersicht!B38,Michi!F:F)</f>
-        <v>0.31944444444444453</v>
+        <v>0.3541666666666668</v>
       </c>
       <c r="F38" s="67">
         <f>SUMIF(Sabrina!B:B,Übersicht!B38,Sabrina!F:F)</f>
-        <v>0.31944444444444453</v>
+        <v>0.3541666666666668</v>
       </c>
       <c r="G38" s="67">
         <f t="shared" si="0"/>
-        <v>1.2777777777777781</v>
+        <v>1.4166666666666672</v>
       </c>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.3">
@@ -12277,23 +12277,23 @@
       </c>
       <c r="C44" s="70">
         <f>SUM(C4:C43)</f>
-        <v>0.78125000000000022</v>
+        <v>0.87847222222222254</v>
       </c>
       <c r="D44" s="70">
         <f t="shared" ref="D44:E44" si="1">SUM(D4:D43)</f>
-        <v>0.60416666666666696</v>
+        <v>0.6805555555555558</v>
       </c>
       <c r="E44" s="70">
         <f t="shared" si="1"/>
-        <v>0.86111111111111127</v>
+        <v>0.93750000000000022</v>
       </c>
       <c r="F44" s="70">
         <f t="shared" ref="F44" si="2">SUM(F4:F43)</f>
-        <v>0.55208333333333348</v>
+        <v>0.76736111111111116</v>
       </c>
       <c r="G44" s="70">
         <f t="shared" si="0"/>
-        <v>2.798611111111112</v>
+        <v>3.2638888888888897</v>
       </c>
     </row>
     <row r="45" spans="2:7" x14ac:dyDescent="0.3">
@@ -12362,10 +12362,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:J116"/>
+  <dimension ref="A1:J117"/>
   <sheetViews>
     <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12418,7 +12418,7 @@
       </c>
       <c r="H2" s="67">
         <f>SUM(F:F)</f>
-        <v>0.78125000000000022</v>
+        <v>0.87847222222222254</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -12452,7 +12452,7 @@
         <v>0.77083333333333337</v>
       </c>
       <c r="F4" s="55">
-        <f t="shared" ref="F4:F36" si="0">E4-D4</f>
+        <f t="shared" ref="F4:F37" si="0">E4-D4</f>
         <v>6.9444444444444531E-2</v>
       </c>
     </row>
@@ -12722,31 +12722,55 @@
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="64"/>
-      <c r="C20" s="75"/>
-      <c r="D20" s="55"/>
-      <c r="E20" s="55"/>
+      <c r="A20" s="71">
+        <v>44125</v>
+      </c>
+      <c r="B20" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="D20" s="55">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="E20" s="55">
+        <v>0.625</v>
+      </c>
       <c r="F20" s="55">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4.166666666666663E-2</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="64"/>
+      <c r="A21" s="71">
+        <v>44112</v>
+      </c>
+      <c r="B21" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="C21" s="19" t="s">
+        <v>98</v>
+      </c>
       <c r="D21" s="55"/>
       <c r="E21" s="55"/>
       <c r="F21" s="55">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.0833333333333332E-2</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" s="64"/>
-      <c r="D22" s="55"/>
-      <c r="E22" s="55"/>
+      <c r="A22" s="64">
+        <v>44127</v>
+      </c>
+      <c r="B22" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="D22" s="55">
+        <v>0.46527777777777773</v>
+      </c>
+      <c r="E22" s="55">
+        <v>0.5</v>
+      </c>
       <c r="F22" s="55">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3.4722222222222265E-2</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -12880,7 +12904,7 @@
       <c r="D37" s="55"/>
       <c r="E37" s="55"/>
       <c r="F37" s="55">
-        <f t="shared" ref="F37:F42" si="1">E37-D37</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -12889,7 +12913,7 @@
       <c r="D38" s="55"/>
       <c r="E38" s="55"/>
       <c r="F38" s="55">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="F38:F43" si="1">E38-D38</f>
         <v>0</v>
       </c>
     </row>
@@ -12934,7 +12958,7 @@
       <c r="D43" s="55"/>
       <c r="E43" s="55"/>
       <c r="F43" s="55">
-        <f t="shared" ref="F43:F60" si="2">E43-D43</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -12943,7 +12967,7 @@
       <c r="D44" s="55"/>
       <c r="E44" s="55"/>
       <c r="F44" s="55">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="F44:F61" si="2">E44-D44</f>
         <v>0</v>
       </c>
     </row>
@@ -13096,7 +13120,7 @@
       <c r="D61" s="55"/>
       <c r="E61" s="55"/>
       <c r="F61" s="55">
-        <f t="shared" ref="F61:F82" si="3">E61-D61</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -13105,7 +13129,7 @@
       <c r="D62" s="55"/>
       <c r="E62" s="55"/>
       <c r="F62" s="55">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="F62:F83" si="3">E62-D62</f>
         <v>0</v>
       </c>
     </row>
@@ -13254,6 +13278,9 @@
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A79" s="64"/>
+      <c r="D79" s="55"/>
+      <c r="E79" s="55"/>
       <c r="F79" s="55">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -13279,13 +13306,13 @@
     </row>
     <row r="83" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F83" s="55">
-        <f t="shared" ref="F83:F116" si="4">E83-D83</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="84" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F84" s="55">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="F84:F117" si="4">E84-D84</f>
         <v>0</v>
       </c>
     </row>
@@ -13477,6 +13504,12 @@
     </row>
     <row r="116" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F116" s="55">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F117" s="55">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -13492,7 +13525,7 @@
   <dimension ref="A1:K105"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="A14" sqref="A14:E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13524,7 +13557,7 @@
       <c r="F1" s="54" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="76"/>
+      <c r="G1" s="75"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="64">
@@ -13549,7 +13582,7 @@
       <c r="G2" s="55"/>
       <c r="H2" s="67">
         <f>SUM(F:F)</f>
-        <v>0.60416666666666685</v>
+        <v>0.6805555555555558</v>
       </c>
       <c r="J2" s="74"/>
       <c r="K2" s="67"/>
@@ -13767,22 +13800,40 @@
       <c r="G13" s="55"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14" s="64"/>
-      <c r="D14" s="55"/>
-      <c r="E14" s="55"/>
+      <c r="A14" s="71">
+        <v>44125</v>
+      </c>
+      <c r="B14" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="D14" s="55">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="E14" s="55">
+        <v>0.625</v>
+      </c>
       <c r="F14" s="55">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4.166666666666663E-2</v>
       </c>
       <c r="G14" s="55"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A15" s="71"/>
-      <c r="D15" s="55"/>
-      <c r="E15" s="55"/>
+      <c r="A15" s="64">
+        <v>44127</v>
+      </c>
+      <c r="B15" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="D15" s="55">
+        <v>0.46527777777777773</v>
+      </c>
+      <c r="E15" s="55">
+        <v>0.5</v>
+      </c>
       <c r="F15" s="55">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3.4722222222222265E-2</v>
       </c>
       <c r="G15" s="55"/>
     </row>
@@ -14504,7 +14555,7 @@
   <dimension ref="A1:K110"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14536,7 +14587,7 @@
       <c r="F1" s="54" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="76"/>
+      <c r="G1" s="75"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="64">
@@ -14561,7 +14612,7 @@
       <c r="G2" s="55"/>
       <c r="H2" s="67">
         <f>SUM(F:F)</f>
-        <v>0.86111111111111138</v>
+        <v>0.93750000000000022</v>
       </c>
       <c r="J2" s="74"/>
       <c r="K2" s="67"/>
@@ -14898,22 +14949,40 @@
       <c r="G20" s="55"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="71"/>
-      <c r="D21" s="55"/>
-      <c r="E21" s="55"/>
+      <c r="A21" s="71">
+        <v>44125</v>
+      </c>
+      <c r="B21" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="D21" s="55">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="E21" s="55">
+        <v>0.625</v>
+      </c>
       <c r="F21" s="55">
-        <f>E21-D21</f>
-        <v>0</v>
+        <f t="shared" ref="F21:F52" si="1">E21-D21</f>
+        <v>4.166666666666663E-2</v>
       </c>
       <c r="G21" s="55"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" s="64"/>
-      <c r="D22" s="55"/>
-      <c r="E22" s="55"/>
+      <c r="A22" s="64">
+        <v>44127</v>
+      </c>
+      <c r="B22" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="D22" s="55">
+        <v>0.46527777777777773</v>
+      </c>
+      <c r="E22" s="55">
+        <v>0.5</v>
+      </c>
       <c r="F22" s="55">
-        <f>E22-D22</f>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>3.4722222222222265E-2</v>
       </c>
       <c r="G22" s="55"/>
     </row>
@@ -14922,7 +14991,7 @@
       <c r="D23" s="55"/>
       <c r="E23" s="55"/>
       <c r="F23" s="55">
-        <f>E23-D23</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G23" s="55"/>
@@ -14932,7 +15001,7 @@
       <c r="D24" s="55"/>
       <c r="E24" s="55"/>
       <c r="F24" s="55">
-        <f>E24-D24</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G24" s="55"/>
@@ -14942,7 +15011,7 @@
       <c r="D25" s="55"/>
       <c r="E25" s="55"/>
       <c r="F25" s="55">
-        <f>E25-D25</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G25" s="55"/>
@@ -14952,7 +15021,7 @@
       <c r="D26" s="55"/>
       <c r="E26" s="55"/>
       <c r="F26" s="55">
-        <f>E26-D26</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G26" s="55"/>
@@ -14962,7 +15031,7 @@
       <c r="D27" s="55"/>
       <c r="E27" s="55"/>
       <c r="F27" s="55">
-        <f>E27-D27</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G27" s="55"/>
@@ -14972,7 +15041,7 @@
       <c r="D28" s="55"/>
       <c r="E28" s="55"/>
       <c r="F28" s="55">
-        <f>E28-D28</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G28" s="55"/>
@@ -14983,7 +15052,7 @@
       <c r="D29" s="55"/>
       <c r="E29" s="55"/>
       <c r="F29" s="55">
-        <f>E29-D29</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G29" s="55"/>
@@ -14993,7 +15062,7 @@
       <c r="D30" s="55"/>
       <c r="E30" s="55"/>
       <c r="F30" s="55">
-        <f>E30-D30</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G30" s="55"/>
@@ -15003,7 +15072,7 @@
       <c r="D31" s="55"/>
       <c r="E31" s="55"/>
       <c r="F31" s="55">
-        <f>E31-D31</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G31" s="55"/>
@@ -15013,7 +15082,7 @@
       <c r="D32" s="55"/>
       <c r="E32" s="55"/>
       <c r="F32" s="55">
-        <f>E32-D32</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G32" s="55"/>
@@ -15023,7 +15092,7 @@
       <c r="D33" s="55"/>
       <c r="E33" s="55"/>
       <c r="F33" s="55">
-        <f>E33-D33</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G33" s="55"/>
@@ -15033,7 +15102,7 @@
       <c r="D34" s="55"/>
       <c r="E34" s="55"/>
       <c r="F34" s="55">
-        <f>E34-D34</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G34" s="55"/>
@@ -15043,7 +15112,7 @@
       <c r="D35" s="55"/>
       <c r="E35" s="55"/>
       <c r="F35" s="55">
-        <f>E35-D35</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G35" s="55"/>
@@ -15053,7 +15122,7 @@
       <c r="D36" s="55"/>
       <c r="E36" s="55"/>
       <c r="F36" s="55">
-        <f>E36-D36</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G36" s="55"/>
@@ -15063,7 +15132,7 @@
       <c r="D37" s="55"/>
       <c r="E37" s="55"/>
       <c r="F37" s="55">
-        <f>E37-D37</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G37" s="55"/>
@@ -15073,7 +15142,7 @@
       <c r="D38" s="55"/>
       <c r="E38" s="55"/>
       <c r="F38" s="55">
-        <f>E38-D38</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G38" s="55"/>
@@ -15083,7 +15152,7 @@
       <c r="D39" s="55"/>
       <c r="E39" s="55"/>
       <c r="F39" s="55">
-        <f>E39-D39</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G39" s="55"/>
@@ -15093,7 +15162,7 @@
       <c r="D40" s="55"/>
       <c r="E40" s="55"/>
       <c r="F40" s="55">
-        <f>E40-D40</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G40" s="55"/>
@@ -15103,7 +15172,7 @@
       <c r="D41" s="55"/>
       <c r="E41" s="55"/>
       <c r="F41" s="55">
-        <f>E41-D41</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G41" s="55"/>
@@ -15113,7 +15182,7 @@
       <c r="D42" s="55"/>
       <c r="E42" s="55"/>
       <c r="F42" s="55">
-        <f>E42-D42</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G42" s="55"/>
@@ -15123,7 +15192,7 @@
       <c r="D43" s="55"/>
       <c r="E43" s="55"/>
       <c r="F43" s="55">
-        <f>E43-D43</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G43" s="55"/>
@@ -15133,7 +15202,7 @@
       <c r="D44" s="55"/>
       <c r="E44" s="55"/>
       <c r="F44" s="55">
-        <f>E44-D44</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G44" s="55"/>
@@ -15143,7 +15212,7 @@
       <c r="D45" s="55"/>
       <c r="E45" s="55"/>
       <c r="F45" s="55">
-        <f>E45-D45</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G45" s="55"/>
@@ -15153,7 +15222,7 @@
       <c r="D46" s="55"/>
       <c r="E46" s="55"/>
       <c r="F46" s="55">
-        <f>E46-D46</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G46" s="55"/>
@@ -15163,7 +15232,7 @@
       <c r="D47" s="55"/>
       <c r="E47" s="55"/>
       <c r="F47" s="55">
-        <f>E47-D47</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G47" s="55"/>
@@ -15171,441 +15240,441 @@
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" s="64"/>
       <c r="F48" s="55">
-        <f>E48-D48</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G48" s="55"/>
     </row>
     <row r="49" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F49" s="55">
-        <f>E49-D49</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G49" s="55"/>
     </row>
     <row r="50" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F50" s="55">
-        <f>E50-D50</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G50" s="55"/>
     </row>
     <row r="51" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F51" s="55">
-        <f>E51-D51</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G51" s="55"/>
     </row>
     <row r="52" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F52" s="55">
-        <f>E52-D52</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G52" s="55"/>
     </row>
     <row r="53" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F53" s="55">
-        <f>E53-D53</f>
+        <f t="shared" ref="F53:F84" si="2">E53-D53</f>
         <v>0</v>
       </c>
       <c r="G53" s="55"/>
     </row>
     <row r="54" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F54" s="55">
-        <f>E54-D54</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G54" s="55"/>
     </row>
     <row r="55" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F55" s="55">
-        <f>E55-D55</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G55" s="55"/>
     </row>
     <row r="56" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F56" s="55">
-        <f>E56-D56</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G56" s="55"/>
     </row>
     <row r="57" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F57" s="55">
-        <f>E57-D57</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G57" s="55"/>
     </row>
     <row r="58" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F58" s="55">
-        <f>E58-D58</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G58" s="55"/>
     </row>
     <row r="59" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F59" s="55">
-        <f>E59-D59</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G59" s="55"/>
     </row>
     <row r="60" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F60" s="55">
-        <f>E60-D60</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G60" s="55"/>
     </row>
     <row r="61" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F61" s="55">
-        <f>E61-D61</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G61" s="55"/>
     </row>
     <row r="62" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F62" s="55">
-        <f>E62-D62</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G62" s="55"/>
     </row>
     <row r="63" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F63" s="55">
-        <f>E63-D63</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G63" s="55"/>
     </row>
     <row r="64" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F64" s="55">
-        <f>E64-D64</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G64" s="55"/>
     </row>
     <row r="65" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F65" s="55">
-        <f>E65-D65</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G65" s="55"/>
     </row>
     <row r="66" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F66" s="55">
-        <f>E66-D66</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G66" s="55"/>
     </row>
     <row r="67" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F67" s="55">
-        <f>E67-D67</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G67" s="55"/>
     </row>
     <row r="68" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F68" s="55">
-        <f>E68-D68</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G68" s="55"/>
     </row>
     <row r="69" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F69" s="55">
-        <f>E69-D69</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G69" s="55"/>
     </row>
     <row r="70" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F70" s="55">
-        <f>E70-D70</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G70" s="55"/>
     </row>
     <row r="71" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F71" s="55">
-        <f>E71-D71</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G71" s="55"/>
     </row>
     <row r="72" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F72" s="55">
-        <f>E72-D72</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G72" s="55"/>
     </row>
     <row r="73" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F73" s="55">
-        <f>E73-D73</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G73" s="55"/>
     </row>
     <row r="74" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F74" s="55">
-        <f>E74-D74</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G74" s="55"/>
     </row>
     <row r="75" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F75" s="55">
-        <f t="shared" ref="F75:F106" si="1">E75-D75</f>
+        <f t="shared" ref="F75:F106" si="3">E75-D75</f>
         <v>0</v>
       </c>
       <c r="G75" s="55"/>
     </row>
     <row r="76" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F76" s="55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G76" s="55"/>
     </row>
     <row r="77" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F77" s="55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G77" s="55"/>
     </row>
     <row r="78" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F78" s="55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G78" s="55"/>
     </row>
     <row r="79" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F79" s="55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G79" s="55"/>
     </row>
     <row r="80" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F80" s="55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G80" s="55"/>
     </row>
     <row r="81" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F81" s="55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G81" s="55"/>
     </row>
     <row r="82" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F82" s="55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G82" s="55"/>
     </row>
     <row r="83" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F83" s="55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G83" s="55"/>
     </row>
     <row r="84" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F84" s="55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G84" s="55"/>
     </row>
     <row r="85" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F85" s="55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G85" s="55"/>
     </row>
     <row r="86" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F86" s="55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G86" s="55"/>
     </row>
     <row r="87" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F87" s="55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G87" s="55"/>
     </row>
     <row r="88" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F88" s="55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G88" s="55"/>
     </row>
     <row r="89" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F89" s="55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G89" s="55"/>
     </row>
     <row r="90" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F90" s="55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G90" s="55"/>
     </row>
     <row r="91" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F91" s="55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G91" s="55"/>
     </row>
     <row r="92" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F92" s="55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G92" s="55"/>
     </row>
     <row r="93" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F93" s="55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G93" s="55"/>
     </row>
     <row r="94" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F94" s="55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G94" s="55"/>
     </row>
     <row r="95" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F95" s="55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G95" s="55"/>
     </row>
     <row r="96" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F96" s="55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G96" s="55"/>
     </row>
     <row r="97" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F97" s="55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G97" s="55"/>
     </row>
     <row r="98" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F98" s="55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G98" s="55"/>
     </row>
     <row r="99" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F99" s="55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G99" s="55"/>
     </row>
     <row r="100" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F100" s="55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G100" s="55"/>
     </row>
     <row r="101" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F101" s="55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G101" s="55"/>
     </row>
     <row r="102" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F102" s="55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G102" s="55"/>
     </row>
     <row r="103" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F103" s="55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G103" s="55"/>
     </row>
     <row r="104" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F104" s="55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G104" s="55"/>
     </row>
     <row r="105" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F105" s="55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G105" s="55"/>
     </row>
     <row r="106" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F106" s="55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G106" s="55"/>
     </row>
     <row r="107" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F107" s="55">
-        <f t="shared" ref="F107:F110" si="2">E107-D107</f>
+        <f t="shared" ref="F107:F110" si="4">E107-D107</f>
         <v>0</v>
       </c>
       <c r="G107" s="55"/>
     </row>
     <row r="108" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F108" s="55">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="G108" s="55"/>
     </row>
     <row r="109" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F109" s="55">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="G109" s="55"/>
     </row>
     <row r="110" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F110" s="55">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -15619,7 +15688,7 @@
   <dimension ref="A1:K104"/>
   <sheetViews>
     <sheetView zoomScale="94" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15651,7 +15720,7 @@
       <c r="F1" s="54" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="76"/>
+      <c r="G1" s="75"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="71">
@@ -15673,7 +15742,7 @@
       <c r="G2" s="55"/>
       <c r="H2" s="67">
         <f>SUM(F:F)</f>
-        <v>0.55208333333333348</v>
+        <v>0.76736111111111116</v>
       </c>
       <c r="J2" s="74"/>
       <c r="K2" s="67"/>
@@ -15905,32 +15974,57 @@
       <c r="G14" s="55"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A15" s="71"/>
-      <c r="D15" s="55"/>
-      <c r="E15" s="55"/>
+      <c r="A15" s="71">
+        <v>44125</v>
+      </c>
+      <c r="B15" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="D15" s="55">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="E15" s="55">
+        <v>0.625</v>
+      </c>
       <c r="F15" s="55">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4.166666666666663E-2</v>
       </c>
       <c r="G15" s="55"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A16" s="64"/>
-      <c r="D16" s="55"/>
-      <c r="E16" s="55"/>
+      <c r="A16" s="64">
+        <v>44127</v>
+      </c>
+      <c r="B16" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="D16" s="55">
+        <v>0.46527777777777773</v>
+      </c>
+      <c r="E16" s="55">
+        <v>0.5</v>
+      </c>
       <c r="F16" s="55">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3.4722222222222265E-2</v>
       </c>
       <c r="G16" s="55"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="64"/>
+      <c r="A17" s="64">
+        <v>44130</v>
+      </c>
+      <c r="B17" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="C17" s="19" t="s">
+        <v>101</v>
+      </c>
       <c r="D17" s="55"/>
       <c r="E17" s="55"/>
       <c r="F17" s="55">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.1388888888888889</v>
       </c>
       <c r="G17" s="55"/>
     </row>

</xml_diff>

<commit_message>
db test testweise implementiert
</commit_message>
<xml_diff>
--- a/doc/Projektablaufplan.xlsx
+++ b/doc/Projektablaufplan.xlsx
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="104">
   <si>
     <t>Erstellen Sie auf diesem Arbeitsblatt ein Gantt-Diagramm.
 Geben Sie den Titel dieses Projekts in Zelle B1 ein. 
@@ -373,6 +373,9 @@
   </si>
   <si>
     <t>Entities mit Michi besprechen</t>
+  </si>
+  <si>
+    <t>Datenbank Test testweise implementiert</t>
   </si>
 </sst>
 </file>
@@ -1517,6 +1520,112 @@
       </fill>
     </dxf>
     <dxf>
+      <numFmt numFmtId="167" formatCode="#,##0_ ;\-#,##0\ "/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="25" formatCode="hh:mm"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="2" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="2" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor theme="2" tint="-9.9948118533890809E-2"/>
@@ -2473,112 +2582,6 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="#,##0_ ;\-#,##0\ "/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="25" formatCode="hh:mm"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="2" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="2" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <border>
         <left style="thin">
           <color theme="0" tint="-0.24994659260841701"/>
@@ -3058,7 +3061,7 @@
                   <c:v>0.3715277777777779</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.2256944444444446</c:v>
+                  <c:v>1.3090277777777779</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.3715277777777779</c:v>
@@ -3896,7 +3899,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3933,17 +3936,17 @@
     <filterColumn colId="8" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="9">
-    <tableColumn id="1" name="Arbeitspaket" totalsRowLabel="Ergebnis" dataDxfId="67" totalsRowDxfId="66"/>
-    <tableColumn id="7" name="Aufwandsschätzung[h]" dataDxfId="65" totalsRowDxfId="64"/>
-    <tableColumn id="8" name="tatsächlicher Aufwand[h]" dataDxfId="63" totalsRowDxfId="62">
+    <tableColumn id="1" name="Arbeitspaket" totalsRowLabel="Ergebnis" dataDxfId="21" totalsRowDxfId="20"/>
+    <tableColumn id="7" name="Aufwandsschätzung[h]" dataDxfId="19" totalsRowDxfId="18"/>
+    <tableColumn id="8" name="tatsächlicher Aufwand[h]" dataDxfId="17" totalsRowDxfId="16">
       <calculatedColumnFormula>IF(VLOOKUP(Meilensteine[[#This Row],[Arbeitspaket]],Übersicht!B:G,7,FALSE)=0,"",VLOOKUP(Meilensteine[[#This Row],[Arbeitspaket]],Übersicht!B:G,7,FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Kategorie" dataDxfId="61" totalsRowDxfId="60"/>
-    <tableColumn id="3" name="Zugewiesen an" dataDxfId="59" totalsRowDxfId="58"/>
+    <tableColumn id="2" name="Kategorie" dataDxfId="15" totalsRowDxfId="14"/>
+    <tableColumn id="3" name="Zugewiesen an" dataDxfId="13" totalsRowDxfId="12"/>
     <tableColumn id="4" name="Fortschritt"/>
-    <tableColumn id="5" name="Start" totalsRowDxfId="57"/>
-    <tableColumn id="9" name="Ende" dataDxfId="56" totalsRowDxfId="55" dataCellStyle="Datum"/>
-    <tableColumn id="6" name="Anzahl Tage" totalsRowFunction="sum" totalsRowDxfId="54"/>
+    <tableColumn id="5" name="Start" totalsRowDxfId="11"/>
+    <tableColumn id="9" name="Ende" dataDxfId="10" totalsRowDxfId="9" dataCellStyle="Datum"/>
+    <tableColumn id="6" name="Anzahl Tage" totalsRowFunction="sum" totalsRowDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="Gantt Table Style" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -4209,7 +4212,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -10187,9 +10190,9 @@
       <c r="C50" s="68">
         <v>0.41666666666666669</v>
       </c>
-      <c r="D50" s="59" t="str">
+      <c r="D50" s="59">
         <f>IF(VLOOKUP(Meilensteine[[#This Row],[Arbeitspaket]],Übersicht!B:G,6,FALSE)=0,"",VLOOKUP(Meilensteine[[#This Row],[Arbeitspaket]],Übersicht!B:G,6,FALSE))</f>
-        <v/>
+        <v>8.3333333333333259E-2</v>
       </c>
       <c r="E50" s="31" t="s">
         <v>11</v>
@@ -10528,7 +10531,7 @@
       </c>
       <c r="D52" s="68">
         <f>SUM(D8:D51)</f>
-        <v>2.2152777777777781</v>
+        <v>2.2986111111111116</v>
       </c>
       <c r="E52" s="69" t="s">
         <v>37</v>
@@ -10539,7 +10542,7 @@
       </c>
       <c r="G52" s="28">
         <f>(Meilensteine[[#This Row],[tatsächlicher Aufwand'[h']]]/Meilensteine[[#This Row],[Aufwandsschätzung'[h']]])</f>
-        <v>0.1536608863198459</v>
+        <v>0.15944123314065517</v>
       </c>
       <c r="H52" s="29"/>
       <c r="I52" s="29"/>
@@ -10773,166 +10776,166 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L4:BO54">
-    <cfRule type="expression" dxfId="53" priority="3">
+    <cfRule type="expression" dxfId="67" priority="3">
       <formula>AND(TODAY()&gt;=L$4,TODAY()&lt;M$4)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L3:AP3">
-    <cfRule type="expression" dxfId="52" priority="9">
+    <cfRule type="expression" dxfId="66" priority="9">
       <formula>L$4&lt;=EOMONTH($L$4,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M3:BO3">
-    <cfRule type="expression" dxfId="51" priority="5">
+    <cfRule type="expression" dxfId="65" priority="5">
       <formula>AND(M$4&lt;=EOMONTH($L$4,2),M$4&gt;EOMONTH($L$4,0),M$4&gt;EOMONTH($L$4,1))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L3:BO3">
-    <cfRule type="expression" dxfId="50" priority="4">
+    <cfRule type="expression" dxfId="64" priority="4">
       <formula>AND(L$4&lt;=EOMONTH($L$4,1),L$4&gt;EOMONTH($L$4,0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L7:BO20 L25:BO30 L34:BO51">
-    <cfRule type="expression" dxfId="49" priority="26" stopIfTrue="1">
+    <cfRule type="expression" dxfId="63" priority="26" stopIfTrue="1">
       <formula>AND($E7="Geringes Risiko",L$4&gt;=$H7,L$4&lt;=$H7+$J7-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="48" priority="45" stopIfTrue="1">
+    <cfRule type="expression" dxfId="62" priority="45" stopIfTrue="1">
       <formula>AND($E7="Hohes Risiko",L$4&gt;=$H7,L$4&lt;=$H7+$J7-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="47" priority="63" stopIfTrue="1">
+    <cfRule type="expression" dxfId="61" priority="63" stopIfTrue="1">
       <formula>AND($E7="Im Plan",L$4&gt;=$H7,L$4&lt;=$H7+$J7-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="46" priority="64" stopIfTrue="1">
+    <cfRule type="expression" dxfId="60" priority="64" stopIfTrue="1">
       <formula>AND($E7="Mittleres Risiko",L$4&gt;=$H7,L$4&lt;=$H7+$J7-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="45" priority="65" stopIfTrue="1">
+    <cfRule type="expression" dxfId="59" priority="65" stopIfTrue="1">
       <formula>AND(LEN($E7)=0,L$4&gt;=$H7,L$4&lt;=$H7+$J7-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L54:BO54">
-    <cfRule type="expression" dxfId="44" priority="73" stopIfTrue="1">
+    <cfRule type="expression" dxfId="58" priority="73" stopIfTrue="1">
       <formula>AND(#REF!="Geringes Risiko",L$4&gt;=#REF!,L$4&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="43" priority="74" stopIfTrue="1">
+    <cfRule type="expression" dxfId="57" priority="74" stopIfTrue="1">
       <formula>AND(#REF!="Hohes Risiko",L$4&gt;=#REF!,L$4&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="42" priority="75" stopIfTrue="1">
+    <cfRule type="expression" dxfId="56" priority="75" stopIfTrue="1">
       <formula>AND(#REF!="Im Plan",L$4&gt;=#REF!,L$4&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="41" priority="76" stopIfTrue="1">
+    <cfRule type="expression" dxfId="55" priority="76" stopIfTrue="1">
       <formula>AND(#REF!="Mittleres Risiko",L$4&gt;=#REF!,L$4&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="40" priority="77" stopIfTrue="1">
+    <cfRule type="expression" dxfId="54" priority="77" stopIfTrue="1">
       <formula>AND(LEN(#REF!)=0,L$4&gt;=#REF!,L$4&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E54">
-    <cfRule type="containsText" dxfId="39" priority="1" operator="containsText" text="OK">
+    <cfRule type="containsText" dxfId="53" priority="1" operator="containsText" text="OK">
       <formula>NOT(ISERROR(SEARCH("OK",E54)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="38" priority="2" operator="containsText" text="FEHLER">
+    <cfRule type="containsText" dxfId="52" priority="2" operator="containsText" text="FEHLER">
       <formula>NOT(ISERROR(SEARCH("FEHLER",E54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L53:BO53">
-    <cfRule type="expression" dxfId="37" priority="246" stopIfTrue="1">
+    <cfRule type="expression" dxfId="51" priority="246" stopIfTrue="1">
       <formula>AND(#REF!="Geringes Risiko",L$4&gt;=#REF!,L$4&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="36" priority="247" stopIfTrue="1">
+    <cfRule type="expression" dxfId="50" priority="247" stopIfTrue="1">
       <formula>AND(#REF!="Hohes Risiko",L$4&gt;=#REF!,L$4&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="35" priority="248" stopIfTrue="1">
+    <cfRule type="expression" dxfId="49" priority="248" stopIfTrue="1">
       <formula>AND(#REF!="Im Plan",L$4&gt;=#REF!,L$4&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="249" stopIfTrue="1">
+    <cfRule type="expression" dxfId="48" priority="249" stopIfTrue="1">
       <formula>AND(#REF!="Mittleres Risiko",L$4&gt;=#REF!,L$4&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="33" priority="250" stopIfTrue="1">
+    <cfRule type="expression" dxfId="47" priority="250" stopIfTrue="1">
       <formula>AND(LEN(#REF!)=0,L$4&gt;=#REF!,L$4&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L24:BO24">
-    <cfRule type="expression" dxfId="32" priority="287" stopIfTrue="1">
+    <cfRule type="expression" dxfId="46" priority="287" stopIfTrue="1">
       <formula>AND($E24="Geringes Risiko",L$4&gt;=$H21,L$4&lt;=$H21+$J24-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="288" stopIfTrue="1">
+    <cfRule type="expression" dxfId="45" priority="288" stopIfTrue="1">
       <formula>AND($E24="Hohes Risiko",L$4&gt;=$H21,L$4&lt;=$H21+$J24-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="289" stopIfTrue="1">
+    <cfRule type="expression" dxfId="44" priority="289" stopIfTrue="1">
       <formula>AND($E24="Im Plan",L$4&gt;=$H21,L$4&lt;=$H21+$J24-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="29" priority="290" stopIfTrue="1">
+    <cfRule type="expression" dxfId="43" priority="290" stopIfTrue="1">
       <formula>AND($E24="Mittleres Risiko",L$4&gt;=$H21,L$4&lt;=$H21+$J24-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="291" stopIfTrue="1">
+    <cfRule type="expression" dxfId="42" priority="291" stopIfTrue="1">
       <formula>AND(LEN($E24)=0,L$4&gt;=$H21,L$4&lt;=$H21+$J24-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L21:BO23">
-    <cfRule type="expression" dxfId="27" priority="351" stopIfTrue="1">
+    <cfRule type="expression" dxfId="41" priority="351" stopIfTrue="1">
       <formula>AND($E21="Geringes Risiko",L$4&gt;=#REF!,L$4&lt;=#REF!+$J21-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="352" stopIfTrue="1">
+    <cfRule type="expression" dxfId="40" priority="352" stopIfTrue="1">
       <formula>AND($E21="Hohes Risiko",L$4&gt;=#REF!,L$4&lt;=#REF!+$J21-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="353" stopIfTrue="1">
+    <cfRule type="expression" dxfId="39" priority="353" stopIfTrue="1">
       <formula>AND($E21="Im Plan",L$4&gt;=#REF!,L$4&lt;=#REF!+$J21-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="354" stopIfTrue="1">
+    <cfRule type="expression" dxfId="38" priority="354" stopIfTrue="1">
       <formula>AND($E21="Mittleres Risiko",L$4&gt;=#REF!,L$4&lt;=#REF!+$J21-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="355" stopIfTrue="1">
+    <cfRule type="expression" dxfId="37" priority="355" stopIfTrue="1">
       <formula>AND(LEN($E21)=0,L$4&gt;=#REF!,L$4&lt;=#REF!+$J21-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L52:BO52">
-    <cfRule type="expression" dxfId="22" priority="406" stopIfTrue="1">
+    <cfRule type="expression" dxfId="36" priority="406" stopIfTrue="1">
       <formula>AND(#REF!="Geringes Risiko",L$4&gt;=#REF!,L$4&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="407" stopIfTrue="1">
+    <cfRule type="expression" dxfId="35" priority="407" stopIfTrue="1">
       <formula>AND(#REF!="Hohes Risiko",L$4&gt;=#REF!,L$4&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="408" stopIfTrue="1">
+    <cfRule type="expression" dxfId="34" priority="408" stopIfTrue="1">
       <formula>AND(#REF!="Im Plan",L$4&gt;=#REF!,L$4&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="409" stopIfTrue="1">
+    <cfRule type="expression" dxfId="33" priority="409" stopIfTrue="1">
       <formula>AND(#REF!="Mittleres Risiko",L$4&gt;=#REF!,L$4&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="410" stopIfTrue="1">
+    <cfRule type="expression" dxfId="32" priority="410" stopIfTrue="1">
       <formula>AND(LEN(#REF!)=0,L$4&gt;=#REF!,L$4&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L31:BO32">
-    <cfRule type="expression" dxfId="17" priority="417" stopIfTrue="1">
+    <cfRule type="expression" dxfId="31" priority="417" stopIfTrue="1">
       <formula>AND($E33="Geringes Risiko",L$4&gt;=$H31,L$4&lt;=$H31+$J31-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="418" stopIfTrue="1">
+    <cfRule type="expression" dxfId="30" priority="418" stopIfTrue="1">
       <formula>AND($E33="Hohes Risiko",L$4&gt;=$H31,L$4&lt;=$H31+$J31-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="419" stopIfTrue="1">
+    <cfRule type="expression" dxfId="29" priority="419" stopIfTrue="1">
       <formula>AND($E33="Im Plan",L$4&gt;=$H31,L$4&lt;=$H31+$J31-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="420" stopIfTrue="1">
+    <cfRule type="expression" dxfId="28" priority="420" stopIfTrue="1">
       <formula>AND($E33="Mittleres Risiko",L$4&gt;=$H31,L$4&lt;=$H31+$J31-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="421" stopIfTrue="1">
+    <cfRule type="expression" dxfId="27" priority="421" stopIfTrue="1">
       <formula>AND(LEN($E33)=0,L$4&gt;=$H31,L$4&lt;=$H31+$J31-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L33:BO33">
-    <cfRule type="expression" dxfId="12" priority="422" stopIfTrue="1">
+    <cfRule type="expression" dxfId="26" priority="422" stopIfTrue="1">
       <formula>AND(#REF!="Geringes Risiko",L$4&gt;=$H33,L$4&lt;=$H33+$J33-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="423" stopIfTrue="1">
+    <cfRule type="expression" dxfId="25" priority="423" stopIfTrue="1">
       <formula>AND(#REF!="Hohes Risiko",L$4&gt;=$H33,L$4&lt;=$H33+$J33-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="424" stopIfTrue="1">
+    <cfRule type="expression" dxfId="24" priority="424" stopIfTrue="1">
       <formula>AND(#REF!="Im Plan",L$4&gt;=$H33,L$4&lt;=$H33+$J33-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="425" stopIfTrue="1">
+    <cfRule type="expression" dxfId="23" priority="425" stopIfTrue="1">
       <formula>AND(#REF!="Mittleres Risiko",L$4&gt;=$H33,L$4&lt;=$H33+$J33-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="426" stopIfTrue="1">
+    <cfRule type="expression" dxfId="22" priority="426" stopIfTrue="1">
       <formula>AND(LEN(#REF!)=0,L$4&gt;=$H33,L$4&lt;=$H33+$J33-1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12000,7 +12003,7 @@
       </c>
       <c r="D40" s="67">
         <f>SUMIF(Roman!B:B,Übersicht!B40,Roman!F:F)</f>
-        <v>0</v>
+        <v>8.3333333333333259E-2</v>
       </c>
       <c r="E40" s="67">
         <f>SUMIF(Michi!B:B,Übersicht!B40,Michi!F:F)</f>
@@ -12012,7 +12015,7 @@
       </c>
       <c r="G40" s="67">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>8.3333333333333259E-2</v>
       </c>
     </row>
     <row r="41" spans="2:7" ht="14.45" x14ac:dyDescent="0.3">
@@ -12097,7 +12100,7 @@
       </c>
       <c r="D44" s="70">
         <f t="shared" ref="D44:E44" si="1">SUM(D4:D43)</f>
-        <v>1.2256944444444446</v>
+        <v>1.3090277777777779</v>
       </c>
       <c r="E44" s="70">
         <f t="shared" si="1"/>
@@ -12109,7 +12112,7 @@
       </c>
       <c r="G44" s="70">
         <f t="shared" si="0"/>
-        <v>2.3402777777777781</v>
+        <v>2.4236111111111116</v>
       </c>
     </row>
     <row r="45" spans="2:7" ht="14.45" x14ac:dyDescent="0.3">
@@ -13142,7 +13145,7 @@
   <dimension ref="A1:K104"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13200,7 +13203,7 @@
       <c r="G2" s="55"/>
       <c r="H2" s="67">
         <f>SUM(F:F)</f>
-        <v>1.2256944444444446</v>
+        <v>1.3090277777777779</v>
       </c>
       <c r="J2" s="74"/>
       <c r="K2" s="67"/>
@@ -13264,7 +13267,7 @@
         <v>0.77083333333333337</v>
       </c>
       <c r="F5" s="55">
-        <f>E5-D5</f>
+        <f t="shared" ref="F5:F13" si="1">E5-D5</f>
         <v>0.125</v>
       </c>
       <c r="G5" s="55"/>
@@ -13283,7 +13286,7 @@
         <v>0.4375</v>
       </c>
       <c r="F6" s="55">
-        <f>E6-D6</f>
+        <f t="shared" si="1"/>
         <v>4.1666666666666685E-2</v>
       </c>
       <c r="G6" s="55"/>
@@ -13302,7 +13305,7 @@
         <v>0.57638888888888895</v>
       </c>
       <c r="F7" s="55">
-        <f>E7-D7</f>
+        <f t="shared" si="1"/>
         <v>4.1666666666666741E-2</v>
       </c>
       <c r="G7" s="55"/>
@@ -13324,7 +13327,7 @@
         <v>0.79166666666666663</v>
       </c>
       <c r="F8" s="55">
-        <f>E8-D8</f>
+        <f t="shared" si="1"/>
         <v>0.11458333333333326</v>
       </c>
       <c r="G8" s="55"/>
@@ -13346,7 +13349,7 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="F9" s="55">
-        <f>E9-D9</f>
+        <f t="shared" si="1"/>
         <v>8.333333333333337E-2</v>
       </c>
       <c r="G9" s="55"/>
@@ -13368,7 +13371,7 @@
         <v>0.95833333333333337</v>
       </c>
       <c r="F10" s="55">
-        <f>E10-D10</f>
+        <f t="shared" si="1"/>
         <v>8.333333333333337E-2</v>
       </c>
       <c r="G10" s="55"/>
@@ -13390,7 +13393,7 @@
         <v>0.89583333333333337</v>
       </c>
       <c r="F11" s="55">
-        <f>E11-D11</f>
+        <f t="shared" si="1"/>
         <v>0.10416666666666674</v>
       </c>
       <c r="G11" s="55"/>
@@ -13412,7 +13415,7 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="F12" s="55">
-        <f>E12-D12</f>
+        <f t="shared" si="1"/>
         <v>0.125</v>
       </c>
       <c r="G12" s="55"/>
@@ -13434,7 +13437,7 @@
         <v>0.72916666666666663</v>
       </c>
       <c r="F13" s="55">
-        <f>E13-D13</f>
+        <f t="shared" si="1"/>
         <v>2.0833333333333259E-2</v>
       </c>
       <c r="G13" s="55"/>
@@ -13525,12 +13528,24 @@
       <c r="G17" s="55"/>
     </row>
     <row r="18" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A18" s="64"/>
-      <c r="D18" s="55"/>
-      <c r="E18" s="55"/>
+      <c r="A18" s="64">
+        <v>44143</v>
+      </c>
+      <c r="B18" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="C18" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="D18" s="55">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="E18" s="55">
+        <v>0.91666666666666663</v>
+      </c>
       <c r="F18" s="55">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>8.3333333333333259E-2</v>
       </c>
       <c r="G18" s="55"/>
     </row>
@@ -13947,258 +13962,258 @@
     </row>
     <row r="68" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F68" s="55">
-        <f t="shared" ref="F68:F104" si="1">E68-D68</f>
+        <f t="shared" ref="F68:F104" si="2">E68-D68</f>
         <v>0</v>
       </c>
       <c r="G68" s="55"/>
     </row>
     <row r="69" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F69" s="55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G69" s="55"/>
     </row>
     <row r="70" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F70" s="55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G70" s="55"/>
     </row>
     <row r="71" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F71" s="55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G71" s="55"/>
     </row>
     <row r="72" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F72" s="55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G72" s="55"/>
     </row>
     <row r="73" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F73" s="55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G73" s="55"/>
     </row>
     <row r="74" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F74" s="55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G74" s="55"/>
     </row>
     <row r="75" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F75" s="55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G75" s="55"/>
     </row>
     <row r="76" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F76" s="55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G76" s="55"/>
     </row>
     <row r="77" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F77" s="55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G77" s="55"/>
     </row>
     <row r="78" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F78" s="55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G78" s="55"/>
     </row>
     <row r="79" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F79" s="55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G79" s="55"/>
     </row>
     <row r="80" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F80" s="55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G80" s="55"/>
     </row>
     <row r="81" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F81" s="55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G81" s="55"/>
     </row>
     <row r="82" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F82" s="55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G82" s="55"/>
     </row>
     <row r="83" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F83" s="55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G83" s="55"/>
     </row>
     <row r="84" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F84" s="55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G84" s="55"/>
     </row>
     <row r="85" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F85" s="55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G85" s="55"/>
     </row>
     <row r="86" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F86" s="55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G86" s="55"/>
     </row>
     <row r="87" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F87" s="55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G87" s="55"/>
     </row>
     <row r="88" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F88" s="55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G88" s="55"/>
     </row>
     <row r="89" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F89" s="55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G89" s="55"/>
     </row>
     <row r="90" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F90" s="55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G90" s="55"/>
     </row>
     <row r="91" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F91" s="55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G91" s="55"/>
     </row>
     <row r="92" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F92" s="55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G92" s="55"/>
     </row>
     <row r="93" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F93" s="55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G93" s="55"/>
     </row>
     <row r="94" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F94" s="55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G94" s="55"/>
     </row>
     <row r="95" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F95" s="55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G95" s="55"/>
     </row>
     <row r="96" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F96" s="55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G96" s="55"/>
     </row>
     <row r="97" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F97" s="55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G97" s="55"/>
     </row>
     <row r="98" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F98" s="55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G98" s="55"/>
     </row>
     <row r="99" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F99" s="55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G99" s="55"/>
     </row>
     <row r="100" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F100" s="55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G100" s="55"/>
     </row>
     <row r="101" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F101" s="55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G101" s="55"/>
     </row>
     <row r="102" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F102" s="55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G102" s="55"/>
     </row>
     <row r="103" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F103" s="55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="104" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F104" s="55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added migration and user data
</commit_message>
<xml_diff>
--- a/doc/Projektablaufplan.xlsx
+++ b/doc/Projektablaufplan.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50020FC2-227E-4220-9180-801F05AA6878}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1A9C0BF-06BB-46C0-BC81-45534941D349}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3945" yWindow="1215" windowWidth="28800" windowHeight="15435" tabRatio="415" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,8 +17,8 @@
     <sheet name="Gantt Info" sheetId="12" r:id="rId7"/>
   </sheets>
   <definedNames>
+    <definedName name="Heute" localSheetId="0">TODAY()</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Gantt!$3:$6</definedName>
-    <definedName name="Heute" localSheetId="0">TODAY()</definedName>
     <definedName name="Projekt_Start">Gantt!$H$2</definedName>
     <definedName name="Scroll_Schrittweite">Gantt!$H$3</definedName>
   </definedNames>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="117">
   <si>
     <t>Erstellen Sie auf diesem Arbeitsblatt ein Gantt-Diagramm.
 Geben Sie den Titel dieses Projekts in Zelle B1 ein. 
@@ -414,6 +414,9 @@
   </si>
   <si>
     <t>Entities überarbeiten</t>
+  </si>
+  <si>
+    <t>Benutzer Daten/ Authorisierung</t>
   </si>
 </sst>
 </file>
@@ -1417,57 +1420,57 @@
     </xf>
   </cellXfs>
   <cellStyles count="52">
-    <cellStyle name="20 % - Akzent1" xfId="28" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent2" xfId="32" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent3" xfId="35" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent4" xfId="39" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent5" xfId="43" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent6" xfId="47" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent1" xfId="29" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent2" xfId="33" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent3" xfId="36" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent4" xfId="40" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent5" xfId="44" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent6" xfId="48" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent1" xfId="30" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent2" xfId="34" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent3" xfId="37" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent4" xfId="41" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent5" xfId="45" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent6" xfId="49" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Akzent1" xfId="27" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Akzent2" xfId="31" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Akzent3" xfId="11" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Akzent4" xfId="38" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Akzent5" xfId="42" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Akzent6" xfId="46" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Ausgabe" xfId="19" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Berechnung" xfId="20" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="28" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="32" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="35" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="39" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="43" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="47" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="29" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="33" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="36" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="40" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="44" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="48" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="30" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="34" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="37" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="41" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="45" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="49" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="27" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="31" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="11" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="38" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="42" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="46" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="16" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="20" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="22" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Comma" xfId="4" builtinId="3" customBuiltin="1"/>
+    <cellStyle name="Comma [0]" xfId="10" builtinId="6" customBuiltin="1"/>
+    <cellStyle name="Currency" xfId="12" builtinId="4" customBuiltin="1"/>
+    <cellStyle name="Currency [0]" xfId="13" builtinId="7" customBuiltin="1"/>
     <cellStyle name="Datum" xfId="9" xr:uid="{00000000-0005-0000-0000-00001A000000}"/>
-    <cellStyle name="Dezimal [0]" xfId="10" builtinId="6" customBuiltin="1"/>
-    <cellStyle name="Eingabe" xfId="18" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Ergebnis" xfId="26" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Erklärender Text" xfId="25" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Gut" xfId="15" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Komma" xfId="4" builtinId="3" customBuiltin="1"/>
-    <cellStyle name="Link" xfId="1" builtinId="8" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="25" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="15" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="6" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="7" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="8" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="14" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="18" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="21" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="17" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Notiz" xfId="24" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Prozent" xfId="2" builtinId="5" customBuiltin="1"/>
-    <cellStyle name="Schlecht" xfId="16" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0" customBuiltin="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
+    <cellStyle name="Note" xfId="24" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="19" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5" customBuiltin="1"/>
     <cellStyle name="Tiefe 1" xfId="50" xr:uid="{00000000-0005-0000-0000-000027000000}"/>
     <cellStyle name="Tiefe 2" xfId="51" xr:uid="{00000000-0005-0000-0000-000028000000}"/>
-    <cellStyle name="Überschrift" xfId="5" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Überschrift 1" xfId="6" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Überschrift 2" xfId="7" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Überschrift 3" xfId="8" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Überschrift 4" xfId="14" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Verknüpfte Zelle" xfId="21" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Währung" xfId="12" builtinId="4" customBuiltin="1"/>
-    <cellStyle name="Währung [0]" xfId="13" builtinId="7" customBuiltin="1"/>
-    <cellStyle name="Warnender Text" xfId="23" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Zelle überprüfen" xfId="22" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="5" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="26" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="23" builtinId="11" customBuiltin="1"/>
     <cellStyle name="zHiddenText" xfId="3" xr:uid="{00000000-0005-0000-0000-000033000000}"/>
   </cellStyles>
   <dxfs count="80">
@@ -2867,7 +2870,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="de-DE"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3093,7 +3096,7 @@
                   <c:v>0.87847222222222254</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.666666666666667</c:v>
+                  <c:v>1.8125000000000004</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.93750000000000022</c:v>
@@ -4270,7 +4273,7 @@
       <selection pane="bottomLeft" activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.7109375" style="14" customWidth="1"/>
     <col min="2" max="2" width="42.5703125" customWidth="1"/>
@@ -7670,7 +7673,7 @@
       </c>
       <c r="D26" s="59">
         <f>IF(VLOOKUP(Meilensteine[[#This Row],[Arbeitspaket]],Übersicht!B:G,6,FALSE)=0,"",VLOOKUP(Meilensteine[[#This Row],[Arbeitspaket]],Übersicht!B:G,6,FALSE))</f>
-        <v>0.25</v>
+        <v>0.39583333333333337</v>
       </c>
       <c r="E26" s="31" t="s">
         <v>11</v>
@@ -10719,7 +10722,7 @@
       </c>
       <c r="D54" s="68">
         <f>SUM(D8:D53)</f>
-        <v>4.2500000000000018</v>
+        <v>4.3958333333333348</v>
       </c>
       <c r="E54" s="69" t="s">
         <v>37</v>
@@ -10730,7 +10733,7 @@
       </c>
       <c r="G54" s="28">
         <f>(Meilensteine[[#This Row],[tatsächlicher Aufwand'[h']]]/Meilensteine[[#This Row],[Aufwandsschätzung'[h']]])</f>
-        <v>0.29479768786127186</v>
+        <v>0.30491329479768803</v>
       </c>
       <c r="H54" s="29"/>
       <c r="I54" s="29"/>
@@ -11277,7 +11280,7 @@
       <selection pane="bottomLeft" activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.28515625" customWidth="1"/>
     <col min="2" max="2" width="44.140625" customWidth="1"/>
@@ -11695,7 +11698,7 @@
       </c>
       <c r="D19" s="67">
         <f>SUMIF(Roman!B:B,Übersicht!B19,Roman!F:F)</f>
-        <v>0.25</v>
+        <v>0.39583333333333337</v>
       </c>
       <c r="E19" s="67">
         <f>SUMIF(Michi!B:B,Übersicht!B19,Michi!F:F)</f>
@@ -11707,7 +11710,7 @@
       </c>
       <c r="G19" s="67">
         <f t="shared" si="0"/>
-        <v>0.25</v>
+        <v>0.39583333333333337</v>
       </c>
     </row>
     <row r="20" spans="2:7" ht="14.45" x14ac:dyDescent="0.3">
@@ -12320,7 +12323,7 @@
       </c>
       <c r="D44" s="70">
         <f t="shared" ref="D44:E44" si="1">SUM(D4:D43)</f>
-        <v>1.666666666666667</v>
+        <v>1.8125000000000004</v>
       </c>
       <c r="E44" s="70">
         <f t="shared" si="1"/>
@@ -12332,7 +12335,7 @@
       </c>
       <c r="G44" s="70">
         <f t="shared" si="0"/>
-        <v>4.25</v>
+        <v>4.3958333333333339</v>
       </c>
     </row>
     <row r="45" spans="2:7" ht="14.45" x14ac:dyDescent="0.3">
@@ -12407,7 +12410,7 @@
       <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.5703125" style="19" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="34.85546875" style="19" bestFit="1" customWidth="1"/>
@@ -13564,10 +13567,10 @@
   <dimension ref="A1:K105"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.5703125" style="19" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.28515625" style="19" customWidth="1"/>
@@ -13621,7 +13624,7 @@
       <c r="G2" s="55"/>
       <c r="H2" s="67">
         <f>SUM(F:F)</f>
-        <v>1.791666666666667</v>
+        <v>1.9375000000000004</v>
       </c>
       <c r="J2" s="74"/>
       <c r="K2" s="67"/>
@@ -14030,9 +14033,9 @@
       <c r="G22" s="55"/>
       <c r="I22" s="67"/>
     </row>
-    <row r="23" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="64">
-        <v>44137</v>
+        <v>44167</v>
       </c>
       <c r="B23" s="19" t="s">
         <v>77</v>
@@ -14053,12 +14056,24 @@
       <c r="G23" s="55"/>
     </row>
     <row r="24" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A24" s="64"/>
-      <c r="D24" s="55"/>
-      <c r="E24" s="55"/>
+      <c r="A24" s="64">
+        <v>44175</v>
+      </c>
+      <c r="B24" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="C24" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="D24" s="55">
+        <v>0.5625</v>
+      </c>
+      <c r="E24" s="55">
+        <v>0.70833333333333337</v>
+      </c>
       <c r="F24" s="55">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.14583333333333337</v>
       </c>
       <c r="G24" s="55"/>
     </row>
@@ -14692,7 +14707,7 @@
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.5703125" style="19" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.140625" style="19" customWidth="1"/>
@@ -15825,7 +15840,7 @@
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.28515625" style="19" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26.85546875" style="19" customWidth="1"/>
@@ -16859,7 +16874,7 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="87.140625" style="10" customWidth="1"/>
     <col min="2" max="16384" width="9.140625" style="8"/>

</xml_diff>